<commit_message>
Initial Commit: Added Excel File
</commit_message>
<xml_diff>
--- a/src/test/resources/GetDataFromContact.xlsx
+++ b/src/test/resources/GetDataFromContact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\Vtiger_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3FD8D0-51D5-4632-932A-DF48BD1A7973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AEFFDB-0385-4F91-884D-9BEF18B1AC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>FirstName</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>samal</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>khanna</t>
   </si>
 </sst>
 </file>
@@ -92,8 +98,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C645575-55E8-44FE-B7BA-E570D02566CA}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
-  <autoFilter ref="A1:B2" xr:uid="{0C645575-55E8-44FE-B7BA-E570D02566CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C645575-55E8-44FE-B7BA-E570D02566CA}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{0C645575-55E8-44FE-B7BA-E570D02566CA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CA468715-EF43-4D3C-86B5-ABCD2AAB09AD}" name="FirstName"/>
     <tableColumn id="2" xr3:uid="{32FB9D61-49F1-4EF2-A874-B40D59A53B44}" name="LastName"/>
@@ -365,9 +371,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -391,6 +399,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>